<commit_message>
More documentation and notes, No API changes.
</commit_message>
<xml_diff>
--- a/IA_CCBS_BANK_SIDE/Position/CCBS_DownloadPositionAndDetails.xlsx
+++ b/IA_CCBS_BANK_SIDE/Position/CCBS_DownloadPositionAndDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aafent\Desktop\IA\Interfaces\IA_CCBS_BANK_SIDE\Position\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aafent\Desktop\IA\InterfacesGitHub\IA_CCBS_BANK_SIDE\Position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE08A7B-F0BB-48B3-B955-BB9CF3FF6FE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F177A10E-ACB1-4977-BAED-6B3805302291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7800" windowWidth="29040" windowHeight="16440" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Response" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Request!$C$2:$F$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Request!$C$2:$F$90</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Response!$C$2:$G$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="237">
   <si>
     <t>Description</t>
   </si>
@@ -552,12 +552,6 @@
     <t>cb_cap_repos</t>
   </si>
   <si>
-    <t>customerCBSId</t>
-  </si>
-  <si>
-    <t>customerCBSCd</t>
-  </si>
-  <si>
     <t>Insurance Company</t>
   </si>
   <si>
@@ -720,9 +714,6 @@
     <t>Last Update</t>
   </si>
   <si>
-    <t>May 2023</t>
-  </si>
-  <si>
     <t>DownloadPositionAndDetails</t>
   </si>
   <si>
@@ -736,6 +727,59 @@
   </si>
   <si>
     <t>i-Apply / Model</t>
+  </si>
+  <si>
+    <t>May 2024</t>
+  </si>
+  <si>
+    <t>It is the account code below the relative mapping is below. For the CurrentAccount, SavingAccount, DepositAccount it is going to be used the code 3 deposit. For CreditCard and DebitCard it is going to be used the code 999 Card
+14	- LETTERS OF GUARANTEE
+18	- SECURITIES
+19	- AGREEMENTS
+20	- COLLATERALS
+3	- DEPOSIT
+37	- TRADE FINANCE
+39	- LETTER OF CREDIT
+4	- LOANS
+80	- NON PROFITS ACCOUNT
+99	- ALL SYSTEM
+999	- CARD</t>
+  </si>
+  <si>
+    <t>It is the account type code, the relative mapping is below.
+3 - Agreements
+5 - Deposits
+6 - Loans</t>
+  </si>
+  <si>
+    <t>Even for closed deals we need the maturity date to be send.</t>
+  </si>
+  <si>
+    <t>It is the currency of the deal with code</t>
+  </si>
+  <si>
+    <t>1 - SHORT TERM CREDIT
+2 - OPEN LOAN
+3 - OPEN LOAN PROMISSORY NOTES
+4 - AMORTIZATION LOAN
+5 - CAPITAL AMORTIZATION LOAN
+6 - OPEN LOAN WITH UNEQUAL INSTALLMENTS
+7 - OPEN CREDIT</t>
+  </si>
+  <si>
+    <t>i-Apply details</t>
+  </si>
+  <si>
+    <t>Is the reference for loans that have been created from i-Apply</t>
+  </si>
+  <si>
+    <t>Entity-Account Type</t>
+  </si>
+  <si>
+    <t>Entity-Account Number</t>
+  </si>
+  <si>
+    <t>Entity-Account Check Digit</t>
   </si>
 </sst>
 </file>
@@ -899,7 +943,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -988,15 +1032,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
     <cellStyle name="60% - Accent4" xfId="2" builtinId="44"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1073,39 +1126,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6ACF92C-1104-4C93-8F8B-A938A4312D3B}" name="Table2" displayName="Table2" ref="B2:F10" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B2:F10" xr:uid="{A6ACF92C-1104-4C93-8F8B-A938A4312D3B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A6ACF92C-1104-4C93-8F8B-A938A4312D3B}" name="Table2" displayName="Table2" ref="B2:F7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="B2:F7" xr:uid="{A6ACF92C-1104-4C93-8F8B-A938A4312D3B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{85C05364-CF34-480B-84A9-1E752A61B8E7}" name="Seq" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{B74F6632-9589-464E-84C1-0830E8F1F8D8}" name="Description" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{9572A906-3602-4DBD-9459-262F500E1D9A}" name="i-Apply / Model" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{88CBB51C-2237-4EBC-90F4-9EFEDD4BEC32}" name="Data Type" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{2E373EFE-D19B-41E5-92FD-B165DCC3E8F5}" name="Notes" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{85C05364-CF34-480B-84A9-1E752A61B8E7}" name="Seq" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{B74F6632-9589-464E-84C1-0830E8F1F8D8}" name="Description" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{9572A906-3602-4DBD-9459-262F500E1D9A}" name="i-Apply / Model" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{88CBB51C-2237-4EBC-90F4-9EFEDD4BEC32}" name="Data Type" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{2E373EFE-D19B-41E5-92FD-B165DCC3E8F5}" name="Notes" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}" name="Table3" displayName="Table3" ref="B2:H100" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B2:H100" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D85FC2E3-79A0-45C2-8639-25646ED6A534}" name="seq" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{83E3CCC0-86B9-42D8-98C9-3A75A9998122}" name="Description" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{33920283-5C7A-4D81-82C6-FC077DC9168F}" name="Model" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}" name="Table3" displayName="Table3" ref="B2:I100" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I100" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D85FC2E3-79A0-45C2-8639-25646ED6A534}" name="seq" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{83E3CCC0-86B9-42D8-98C9-3A75A9998122}" name="Description" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{33920283-5C7A-4D81-82C6-FC077DC9168F}" name="Model" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{21207700-9C5E-49FF-B1F1-B3E80983459F}" name="iApply" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{AEB71BB6-2882-4936-9A74-CF7DC5A067E2}" name="Data Type" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{EE278FB3-8A4A-41A3-82EB-96E212089493}" name="Entity" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{14553218-EA08-43B1-8723-80FF07BE96F7}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{EC9AF9B7-009D-464A-B823-D133DBB7F12A}" name="i-Apply details" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1143,7 +1197,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1249,7 +1303,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1391,7 +1445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1401,104 +1455,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB8ACDA-C8F4-4728-9499-8B46BAA74AEA}">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
@@ -1509,41 +1561,41 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03AC1DB5-1548-45C4-B0E5-7097191C5328}">
-  <dimension ref="B2:F91"/>
+  <dimension ref="B2:F88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="12.7109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="56.140625" style="21" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="4.109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="56.109375" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="23">
         <v>1</v>
       </c>
@@ -1558,7 +1610,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="23">
         <v>2</v>
       </c>
@@ -1573,12 +1625,12 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>234</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -1590,12 +1642,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -1607,12 +1659,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="23">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>236</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1624,562 +1676,517 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="25">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="25">
-        <v>8</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="24"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="9"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="24"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="9"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="24"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
+    <row r="17" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="22"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="2:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="24"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="24"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="24"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="24"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B26" s="24"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="24"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="24"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="8"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B29" s="24"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="24"/>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="24"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="25"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="25"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="25"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B34" s="25"/>
       <c r="C34" s="12"/>
       <c r="D34" s="13"/>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B35" s="25"/>
       <c r="C35" s="12"/>
       <c r="D35" s="13"/>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B36" s="25"/>
       <c r="C36" s="12"/>
       <c r="D36" s="13"/>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="12"/>
-    </row>
-    <row r="38" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="25"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="12"/>
-    </row>
-    <row r="39" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="25"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="24"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="2:6" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="26"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="15"/>
       <c r="F40" s="14"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="24"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="2:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="26"/>
+    <row r="41" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="25"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="25"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="15"/>
       <c r="F43" s="14"/>
     </row>
-    <row r="44" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="25"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="14"/>
-    </row>
-    <row r="45" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="14"/>
-    </row>
-    <row r="46" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="25"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="17"/>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="17"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="24"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="8"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="8"/>
-    </row>
-    <row r="52" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="24"/>
+    <row r="50" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="24"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="24"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="24"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="14"/>
-    </row>
-    <row r="54" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="24"/>
+    <row r="53" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="15"/>
       <c r="F54" s="14"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
       <c r="F55" s="8"/>
     </row>
-    <row r="56" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="9"/>
-      <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="14"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="19"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="19"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="8"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F58" s="19"/>
+    </row>
+    <row r="59" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="24"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
-      <c r="F59" s="19"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="24"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="19"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="24"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="19"/>
-    </row>
-    <row r="62" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="24"/>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="9"/>
       <c r="F62" s="8"/>
     </row>
-    <row r="63" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="24"/>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="8"/>
     </row>
-    <row r="64" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="24"/>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
       <c r="E64" s="9"/>
       <c r="F64" s="8"/>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="8"/>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="9"/>
       <c r="F66" s="8"/>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="9"/>
       <c r="F67" s="8"/>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="9"/>
       <c r="F68" s="8"/>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="9"/>
       <c r="F70" s="8"/>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
       <c r="F71" s="8"/>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="9"/>
       <c r="F72" s="8"/>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="8"/>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="9"/>
-      <c r="F74" s="8"/>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="12"/>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
-      <c r="F75" s="8"/>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="12"/>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="9"/>
-      <c r="F76" s="8"/>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="9"/>
-      <c r="F77" s="12"/>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="9"/>
-      <c r="F78" s="12"/>
-    </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="9"/>
-      <c r="F79" s="12"/>
-    </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F79" s="8"/>
+    </row>
+    <row r="80" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="9"/>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="9"/>
       <c r="F81" s="8"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="9"/>
-      <c r="F82" s="8"/>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="24"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="14"/>
+    </row>
+    <row r="83" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="24"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="9"/>
       <c r="F83" s="8"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="24"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="9"/>
       <c r="F84" s="8"/>
     </row>
-    <row r="85" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="24"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="14"/>
-    </row>
-    <row r="86" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="24"/>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="9"/>
       <c r="F86" s="8"/>
     </row>
-    <row r="87" spans="2:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="24"/>
+    <row r="87" spans="2:6" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="27"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="9"/>
       <c r="F87" s="8"/>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="9"/>
       <c r="F88" s="8"/>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="9"/>
-      <c r="F89" s="8"/>
-    </row>
-    <row r="90" spans="2:6" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="27"/>
-      <c r="C90" s="8"/>
-      <c r="D90" s="8"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="8"/>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2191,35 +2198,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DEFA5D-C6DF-4BEE-A0BF-87172BA2BD41}">
-  <dimension ref="B1:H104"/>
+  <dimension ref="B1:J104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="148" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="24" style="1"/>
+    <col min="2" max="2" width="7.109375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="66.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="24" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:10" s="28" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -2228,13 +2236,16 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="29">
         <v>1</v>
       </c>
@@ -2248,10 +2259,13 @@
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H3" s="30"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="29">
         <v>2</v>
       </c>
@@ -2265,10 +2279,13 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="29">
         <v>3</v>
       </c>
@@ -2282,10 +2299,13 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="29">
         <v>4</v>
       </c>
@@ -2299,10 +2319,13 @@
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="29">
         <v>5</v>
       </c>
@@ -2316,10 +2339,13 @@
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H7" s="30"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" ht="216" x14ac:dyDescent="0.3">
       <c r="B8" s="29">
         <v>6</v>
       </c>
@@ -2333,10 +2359,15 @@
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" s="29">
         <v>7</v>
       </c>
@@ -2350,10 +2381,15 @@
         <v>33</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="29">
         <v>8</v>
       </c>
@@ -2367,10 +2403,13 @@
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H10" s="30"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="29">
         <v>9</v>
       </c>
@@ -2384,10 +2423,13 @@
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="29">
         <v>10</v>
       </c>
@@ -2401,13 +2443,15 @@
         <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H12" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" s="30" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="31"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="29">
         <v>11</v>
       </c>
@@ -2421,10 +2465,13 @@
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="29">
         <v>12</v>
       </c>
@@ -2438,10 +2485,13 @@
         <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="29">
         <v>13</v>
       </c>
@@ -2455,10 +2505,13 @@
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="29">
         <v>14</v>
       </c>
@@ -2472,10 +2525,13 @@
         <v>41</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="29">
         <v>15</v>
       </c>
@@ -2489,10 +2545,13 @@
         <v>41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="29">
         <v>16</v>
       </c>
@@ -2506,10 +2565,13 @@
         <v>41</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="29">
         <v>17</v>
       </c>
@@ -2523,10 +2585,13 @@
         <v>41</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="29">
         <v>18</v>
       </c>
@@ -2540,10 +2605,13 @@
         <v>41</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="29">
         <v>19</v>
       </c>
@@ -2557,10 +2625,13 @@
         <v>59</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B22" s="29">
         <v>20</v>
       </c>
@@ -2574,13 +2645,17 @@
         <v>59</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H22" s="30" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" s="29">
         <v>21</v>
       </c>
@@ -2594,13 +2669,17 @@
         <v>20</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H23" s="30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="31" t="s">
+        <v>233</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" s="29">
         <v>22</v>
       </c>
@@ -2614,10 +2693,13 @@
         <v>41</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" s="29">
         <v>23</v>
       </c>
@@ -2631,13 +2713,15 @@
         <v>41</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H25" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H25" s="30" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="31"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" s="29">
         <v>24</v>
       </c>
@@ -2651,10 +2735,13 @@
         <v>41</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="29">
         <v>25</v>
       </c>
@@ -2668,10 +2755,13 @@
         <v>73</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" s="29">
         <v>26</v>
       </c>
@@ -2685,13 +2775,15 @@
         <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H28" s="30" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="31"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B29" s="29">
         <v>27</v>
       </c>
@@ -2705,13 +2797,15 @@
         <v>33</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H29" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H29" s="30" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="31"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" s="29">
         <v>28</v>
       </c>
@@ -2725,10 +2819,13 @@
         <v>20</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B31" s="29">
         <v>29</v>
       </c>
@@ -2742,10 +2839,13 @@
         <v>33</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="H31" s="30"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" s="29">
         <v>30</v>
       </c>
@@ -2759,10 +2859,13 @@
         <v>41</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="H32" s="30"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="29">
         <v>31</v>
       </c>
@@ -2776,10 +2879,13 @@
         <v>41</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="H33" s="30"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="29">
         <v>32</v>
       </c>
@@ -2793,10 +2899,15 @@
         <v>33</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="H34" s="30"/>
+      <c r="I34" s="31" t="s">
+        <v>230</v>
+      </c>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="29">
         <v>33</v>
       </c>
@@ -2810,13 +2921,15 @@
         <v>33</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H35" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H35" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="31"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="2:10" ht="216" x14ac:dyDescent="0.3">
       <c r="B36" s="29">
         <v>34</v>
       </c>
@@ -2830,13 +2943,17 @@
         <v>20</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H36" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H36" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="29">
         <v>35</v>
       </c>
@@ -2850,13 +2967,15 @@
         <v>41</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H37" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H37" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="31"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="29">
         <v>36</v>
       </c>
@@ -2870,13 +2989,15 @@
         <v>41</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H38" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H38" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="31"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="29">
         <v>37</v>
       </c>
@@ -2890,13 +3011,15 @@
         <v>20</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H39" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="31"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="29">
         <v>38</v>
       </c>
@@ -2910,13 +3033,15 @@
         <v>59</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H40" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="31"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="29">
         <v>39</v>
       </c>
@@ -2930,13 +3055,15 @@
         <v>41</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H41" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="31"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="29">
         <v>40</v>
       </c>
@@ -2950,13 +3077,15 @@
         <v>8</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H42" s="30" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="31"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="29">
         <v>41</v>
       </c>
@@ -2970,13 +3099,15 @@
         <v>41</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H43" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H43" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="31"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="29">
         <v>42</v>
       </c>
@@ -2990,13 +3121,15 @@
         <v>41</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H44" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H44" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="31"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="29">
         <v>43</v>
       </c>
@@ -3010,13 +3143,15 @@
         <v>41</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H45" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H45" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="31"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" s="29">
         <v>44</v>
       </c>
@@ -3030,13 +3165,15 @@
         <v>41</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H46" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H46" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="31"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" s="29">
         <v>45</v>
       </c>
@@ -3050,13 +3187,15 @@
         <v>41</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H47" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H47" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="31"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="29">
         <v>46</v>
       </c>
@@ -3070,13 +3209,15 @@
         <v>41</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H48" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H48" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="31"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" s="29">
         <v>47</v>
       </c>
@@ -3090,13 +3231,15 @@
         <v>41</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H49" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H49" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="31"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B50" s="29">
         <v>48</v>
       </c>
@@ -3110,13 +3253,17 @@
         <v>20</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H50" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H50" s="30" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="29">
         <v>49</v>
       </c>
@@ -3130,13 +3277,15 @@
         <v>33</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H51" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H51" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="31"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" s="29">
         <v>50</v>
       </c>
@@ -3150,13 +3299,15 @@
         <v>41</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H52" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="30"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" s="29">
         <v>51</v>
       </c>
@@ -3170,13 +3321,15 @@
         <v>41</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H53" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="30"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" s="29">
         <v>52</v>
       </c>
@@ -3190,13 +3343,15 @@
         <v>41</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H54" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H54" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="30"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" s="29">
         <v>53</v>
       </c>
@@ -3210,13 +3365,15 @@
         <v>41</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H55" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="30"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B56" s="29">
         <v>54</v>
       </c>
@@ -3230,13 +3387,15 @@
         <v>41</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H56" s="30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="30"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" s="29">
         <v>55</v>
       </c>
@@ -3250,13 +3409,15 @@
         <v>33</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H57" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H57" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="30"/>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" s="29">
         <v>56</v>
       </c>
@@ -3270,13 +3431,15 @@
         <v>41</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H58" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H58" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="30"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" s="29">
         <v>57</v>
       </c>
@@ -3290,13 +3453,15 @@
         <v>41</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H59" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H59" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="30"/>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B60" s="29">
         <v>58</v>
       </c>
@@ -3310,13 +3475,15 @@
         <v>41</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H60" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="30"/>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B61" s="29">
         <v>59</v>
       </c>
@@ -3330,13 +3497,15 @@
         <v>41</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H61" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H61" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="30"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B62" s="29">
         <v>60</v>
       </c>
@@ -3350,13 +3519,15 @@
         <v>41</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H62" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H62" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="30"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B63" s="29">
         <v>61</v>
       </c>
@@ -3370,13 +3541,15 @@
         <v>20</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H63" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H63" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="30"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="29">
         <v>62</v>
       </c>
@@ -3390,13 +3563,15 @@
         <v>20</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H64" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H64" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="30"/>
+      <c r="J64" s="1"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65" s="29">
         <v>63</v>
       </c>
@@ -3410,13 +3585,15 @@
         <v>41</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H65" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H65" s="30" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="30"/>
+      <c r="J65" s="1"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" s="29">
         <v>64</v>
       </c>
@@ -3430,13 +3607,15 @@
         <v>33</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H66" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H66" s="30" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="30"/>
+      <c r="J66" s="1"/>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" s="29">
         <v>65</v>
       </c>
@@ -3450,13 +3629,15 @@
         <v>41</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H67" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H67" s="30" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="30"/>
+      <c r="J67" s="1"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="29">
         <v>66</v>
       </c>
@@ -3470,13 +3651,15 @@
         <v>20</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H68" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H68" s="30" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="30"/>
+      <c r="J68" s="1"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" s="29">
         <v>67</v>
       </c>
@@ -3490,13 +3673,15 @@
         <v>41</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H69" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H69" s="30" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="30"/>
+      <c r="J69" s="1"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" s="29">
         <v>68</v>
       </c>
@@ -3510,13 +3695,15 @@
         <v>20</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H70" s="30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="30"/>
+      <c r="J70" s="1"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B71" s="29">
         <v>69</v>
       </c>
@@ -3530,13 +3717,15 @@
         <v>33</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H71" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H71" s="30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="30"/>
+      <c r="J71" s="1"/>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B72" s="29">
         <v>70</v>
       </c>
@@ -3550,13 +3739,15 @@
         <v>41</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H72" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H72" s="30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="30"/>
+      <c r="J72" s="1"/>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B73" s="29">
         <v>71</v>
       </c>
@@ -3570,13 +3761,15 @@
         <v>41</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H73" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H73" s="30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="30"/>
+      <c r="J73" s="1"/>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" s="29">
         <v>72</v>
       </c>
@@ -3590,13 +3783,15 @@
         <v>41</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H74" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H74" s="30" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="30"/>
+      <c r="J74" s="1"/>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" s="29">
         <v>73</v>
       </c>
@@ -3610,13 +3805,14 @@
         <v>20</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H75" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H75" s="30" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J75" s="1"/>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B76" s="29">
         <v>74</v>
       </c>
@@ -3630,13 +3826,14 @@
         <v>41</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H76" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H76" s="30" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J76" s="1"/>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B77" s="29">
         <v>75</v>
       </c>
@@ -3650,13 +3847,14 @@
         <v>41</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H77" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H77" s="30" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J77" s="1"/>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B78" s="29">
         <v>76</v>
       </c>
@@ -3670,13 +3868,14 @@
         <v>41</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H78" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H78" s="30" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J78" s="1"/>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B79" s="29">
         <v>77</v>
       </c>
@@ -3690,13 +3889,14 @@
         <v>41</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H79" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="H79" s="30" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="J79" s="1"/>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B80" s="29">
         <v>78</v>
       </c>
@@ -3710,44 +3910,50 @@
         <v>41</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="H80" s="30"/>
+      <c r="J80" s="1"/>
+    </row>
+    <row r="81" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B81" s="29">
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H81" s="30"/>
+      <c r="J81" s="1"/>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B82" s="29">
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="G82" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H82" s="30"/>
+      <c r="J82" s="1"/>
+    </row>
+    <row r="83" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B83" s="29">
         <v>81</v>
       </c>
@@ -3755,19 +3961,20 @@
         <v>71</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H83" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="J83" s="1"/>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B84" s="29">
         <v>82</v>
       </c>
@@ -3781,13 +3988,14 @@
         <v>8</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H84" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="J84" s="1"/>
+    </row>
+    <row r="85" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B85" s="29">
         <v>83</v>
       </c>
@@ -3801,13 +4009,14 @@
         <v>14</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H85" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="J85" s="1"/>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B86" s="29">
         <v>84</v>
       </c>
@@ -3815,16 +4024,18 @@
         <v>71</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H86" s="30"/>
+      <c r="J86" s="1"/>
+    </row>
+    <row r="87" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B87" s="29">
         <v>85</v>
       </c>
@@ -3832,203 +4043,227 @@
         <v>81</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H87" s="30"/>
+      <c r="J87" s="1"/>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B88" s="29">
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H88" s="30"/>
+      <c r="J88" s="1"/>
+    </row>
+    <row r="89" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B89" s="29">
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H89" s="30"/>
+      <c r="J89" s="1"/>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B90" s="29">
         <v>88</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H90" s="30"/>
+      <c r="J90" s="1"/>
+    </row>
+    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B91" s="29">
         <v>89</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H91" s="30"/>
+      <c r="J91" s="1"/>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B92" s="29">
         <v>90</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H92" s="30"/>
+      <c r="J92" s="1"/>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B93" s="29">
         <v>91</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H93" s="30"/>
+      <c r="J93" s="1"/>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B94" s="29">
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H94" s="30"/>
+      <c r="J94" s="1"/>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B95" s="29">
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H95" s="30"/>
+      <c r="J95" s="1"/>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B96" s="29">
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H96" s="30"/>
+      <c r="J96" s="1"/>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97" s="29">
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H97" s="30"/>
+      <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B98" s="29">
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H98" s="30"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B99" s="29">
         <v>97</v>
       </c>
@@ -4036,33 +4271,37 @@
         <v>36</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="H99" s="30"/>
+      <c r="J99" s="1"/>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B100" s="29">
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="G100" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>207</v>
+      </c>
+      <c r="H100" s="30"/>
+      <c r="J100" s="1"/>
+    </row>
+    <row r="104" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes on DownloadPositionAndDetails API response
</commit_message>
<xml_diff>
--- a/IA_CCBS_BANK_SIDE/Position/CCBS_DownloadPositionAndDetails.xlsx
+++ b/IA_CCBS_BANK_SIDE/Position/CCBS_DownloadPositionAndDetails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aafent\Desktop\IA\InterfacesGitHub\IA_CCBS_BANK_SIDE\Position\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Deploy\IA\InterfacesGitHub\IA_CCBS_BANK_SIDE\Position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F177A10E-ACB1-4977-BAED-6B3805302291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8030FD8E-7A8B-43EF-9685-3BA1C6DF6B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Request!$C$2:$F$90</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Response!$C$2:$G$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Response!$C$2:$G$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="242">
   <si>
     <t>Description</t>
   </si>
@@ -277,17 +277,9 @@
     <t>For all the banks except HF</t>
   </si>
   <si>
-    <t>Account Status</t>
-  </si>
-  <si>
     <t>cb_status</t>
   </si>
   <si>
-    <t>If cb_accd = 3 then code from grp =G0223
-If cb_accd = 5 then code from grp =G0221
-If cb_accd = 6 then code from grp =G0222</t>
-  </si>
-  <si>
     <t>Customer Id</t>
   </si>
   <si>
@@ -444,15 +436,9 @@
     <t>Letter of Guarantee (accountType = 14)</t>
   </si>
   <si>
-    <t>LG Limit Amount</t>
-  </si>
-  <si>
     <t>cb_lg_lmt_amt</t>
   </si>
   <si>
-    <t>LG Commissions Balance</t>
-  </si>
-  <si>
     <t>cb_lg_com_bal</t>
   </si>
   <si>
@@ -462,9 +448,6 @@
     <t>cb_lg_fr_amt</t>
   </si>
   <si>
-    <t>LG Expenses Balance</t>
-  </si>
-  <si>
     <t>cb_lg_exp_bal</t>
   </si>
   <si>
@@ -474,15 +457,9 @@
     <t>cb_lg_amt</t>
   </si>
   <si>
-    <t>LG Expiry Type</t>
-  </si>
-  <si>
     <t>cb_exp_type</t>
   </si>
   <si>
-    <t>LG Obligation Status</t>
-  </si>
-  <si>
     <t>cb_lg_obl_status</t>
   </si>
   <si>
@@ -490,33 +467,6 @@
   </si>
   <si>
     <t>cb_lg_req_amt</t>
-  </si>
-  <si>
-    <t>Trade Finance (accountType = 37)</t>
-  </si>
-  <si>
-    <t>TF Used Amount</t>
-  </si>
-  <si>
-    <t>TF Expiry Type</t>
-  </si>
-  <si>
-    <t>TF Amount</t>
-  </si>
-  <si>
-    <t>Letter of Credit (accountType = 39)</t>
-  </si>
-  <si>
-    <t>LC Limit Amount</t>
-  </si>
-  <si>
-    <t>LC Initial Amount</t>
-  </si>
-  <si>
-    <t>LC Total Issued Amount</t>
-  </si>
-  <si>
-    <t>LC Obligation Status</t>
   </si>
   <si>
     <t>Capital in Market Funds</t>
@@ -780,6 +730,83 @@
   </si>
   <si>
     <t>Entity-Account Check Digit</t>
+  </si>
+  <si>
+    <t>Insurances array</t>
+  </si>
+  <si>
+    <t>Obligation Status (LC, LG)</t>
+  </si>
+  <si>
+    <t>Securities (accountType = 18)
+Letter of Guarantee (accountType = 14)</t>
+  </si>
+  <si>
+    <t>Agreement (accounType = 19)
+Deposit (accountType = 3)
+Letter of Guarantee (accountType = 14)
+Trade Finance (accountType = 37)
+Letter of Credit (accountType = 39)</t>
+  </si>
+  <si>
+    <t>cb_status1</t>
+  </si>
+  <si>
+    <t>varchar(200)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long status </t>
+  </si>
+  <si>
+    <t>Not used</t>
+  </si>
+  <si>
+    <t>Status description</t>
+  </si>
+  <si>
+    <t>Account Category Status</t>
+  </si>
+  <si>
+    <t>Entity (Account) Type Status</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>If cb_accd = 3 then code from grp =G0223 [Closed,Deleted]
+If cb_accd = 5 then code from grp =G0221 [Blocked]
+If cb_accd = 6 then code from grp =G0222 [xfer to bad dept]</t>
+  </si>
+  <si>
+    <t>3 - Agreements
+5 - Deposits
+6 - Loans
+(on comas the buf field has the value of 3,5 or 6)
+Mapped value via cb_accd from coded items: G0223,G0221,G0222 using as key the value of cb_status (see cb_status model field)</t>
+  </si>
+  <si>
+    <t>Valid values are: DELETED, ACTIVE and more (for more values ask us)</t>
+  </si>
+  <si>
+    <t>Letter of Guarantee (accountType = 14)
+Trade Finance (accountType = 37)
+Letter of Credit (accountType = 39)</t>
+  </si>
+  <si>
+    <t>Expiration Type</t>
+  </si>
+  <si>
+    <t>Letter of Guarantee (accountType = 14)
+Letter of Credit (accountType = 39)</t>
+  </si>
+  <si>
+    <t>Entity Commission Balance</t>
+  </si>
+  <si>
+    <t>Entity's Limit Amount</t>
+  </si>
+  <si>
+    <t>Entity's Expenses Balance</t>
   </si>
 </sst>
 </file>
@@ -943,7 +970,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1038,6 +1065,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
@@ -1045,6 +1078,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1062,12 +1101,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1140,17 +1173,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}" name="Table3" displayName="Table3" ref="B2:I100" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I100" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}" name="Table3" displayName="Table3" ref="B2:I89" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I89" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D85FC2E3-79A0-45C2-8639-25646ED6A534}" name="seq" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{83E3CCC0-86B9-42D8-98C9-3A75A9998122}" name="Description" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{33920283-5C7A-4D81-82C6-FC077DC9168F}" name="Model" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{21207700-9C5E-49FF-B1F1-B3E80983459F}" name="iApply" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{AEB71BB6-2882-4936-9A74-CF7DC5A067E2}" name="Data Type" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{EE278FB3-8A4A-41A3-82EB-96E212089493}" name="Entity" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{14553218-EA08-43B1-8723-80FF07BE96F7}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{EC9AF9B7-009D-464A-B823-D133DBB7F12A}" name="i-Apply details" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D85FC2E3-79A0-45C2-8639-25646ED6A534}" name="seq" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{83E3CCC0-86B9-42D8-98C9-3A75A9998122}" name="Description" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{33920283-5C7A-4D81-82C6-FC077DC9168F}" name="Model" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{21207700-9C5E-49FF-B1F1-B3E80983459F}" name="iApply" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{AEB71BB6-2882-4936-9A74-CF7DC5A067E2}" name="Data Type" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{EE278FB3-8A4A-41A3-82EB-96E212089493}" name="Entity" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{14553218-EA08-43B1-8723-80FF07BE96F7}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{EC9AF9B7-009D-464A-B823-D133DBB7F12A}" name="i-Apply details" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1472,34 +1505,34 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
@@ -1508,10 +1541,10 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
@@ -1520,18 +1553,18 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -1544,10 +1577,10 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
@@ -1563,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03AC1DB5-1548-45C4-B0E5-7097191C5328}">
   <dimension ref="B2:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1580,19 +1613,19 @@
   <sheetData>
     <row r="2" spans="2:6" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -1630,7 +1663,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -1647,7 +1680,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -1664,7 +1697,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -2198,9 +2231,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DEFA5D-C6DF-4BEE-A0BF-87172BA2BD41}">
-  <dimension ref="B1:J104"/>
+  <dimension ref="B1:J92"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2221,13 +2256,13 @@
     </row>
     <row r="2" spans="2:10" s="28" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -2236,13 +2271,13 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -2259,7 +2294,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="28"/>
@@ -2279,7 +2314,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -2299,7 +2334,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H5" s="30"/>
       <c r="I5" s="31"/>
@@ -2319,7 +2354,7 @@
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="31"/>
@@ -2339,7 +2374,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="31"/>
@@ -2359,11 +2394,11 @@
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="31" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -2374,18 +2409,18 @@
       <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="32" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H9" s="30"/>
       <c r="I9" s="31" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -2403,7 +2438,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H10" s="30"/>
       <c r="I10" s="31"/>
@@ -2423,7 +2458,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H11" s="30"/>
       <c r="I11" s="31"/>
@@ -2443,7 +2478,7 @@
         <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>38</v>
@@ -2465,7 +2500,7 @@
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="31"/>
@@ -2485,7 +2520,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="31"/>
@@ -2505,7 +2540,7 @@
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="31"/>
@@ -2525,7 +2560,7 @@
         <v>41</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H16" s="30"/>
       <c r="I16" s="31"/>
@@ -2545,7 +2580,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H17" s="30"/>
       <c r="I17" s="31"/>
@@ -2565,7 +2600,7 @@
         <v>41</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H18" s="30"/>
       <c r="I18" s="31"/>
@@ -2585,7 +2620,7 @@
         <v>41</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H19" s="30"/>
       <c r="I19" s="31"/>
@@ -2605,7 +2640,7 @@
         <v>41</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H20" s="30"/>
       <c r="I20" s="31"/>
@@ -2625,7 +2660,7 @@
         <v>59</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H21" s="30"/>
       <c r="I21" s="31"/>
@@ -2645,17 +2680,17 @@
         <v>59</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H22" s="30" t="s">
         <v>62</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B23" s="29">
         <v>21</v>
       </c>
@@ -2669,13 +2704,13 @@
         <v>20</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H23" s="30" t="s">
         <v>65</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="J23" s="1"/>
     </row>
@@ -2693,7 +2728,7 @@
         <v>41</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H24" s="30"/>
       <c r="I24" s="31"/>
@@ -2713,7 +2748,7 @@
         <v>41</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H25" s="30" t="s">
         <v>70</v>
@@ -2735,7 +2770,7 @@
         <v>41</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H26" s="30"/>
       <c r="I26" s="31"/>
@@ -2755,7 +2790,7 @@
         <v>73</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H27" s="30"/>
       <c r="I27" s="31"/>
@@ -2775,7 +2810,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H28" s="30" t="s">
         <v>75</v>
@@ -2783,26 +2818,31 @@
       <c r="I28" s="31"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B29" s="29">
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" s="31"/>
+        <v>233</v>
+      </c>
+      <c r="I29" s="31" t="s">
+        <v>234</v>
+      </c>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
@@ -2810,16 +2850,16 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H30" s="30"/>
       <c r="I30" s="31"/>
@@ -2830,16 +2870,16 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H31" s="30"/>
       <c r="I31" s="31"/>
@@ -2850,16 +2890,16 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H32" s="30"/>
       <c r="I32" s="31"/>
@@ -2870,16 +2910,16 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H33" s="30"/>
       <c r="I33" s="31"/>
@@ -2899,34 +2939,36 @@
         <v>33</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H34" s="30"/>
       <c r="I34" s="31" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B35" s="29">
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="31"/>
+        <v>224</v>
+      </c>
+      <c r="I35" s="31" t="s">
+        <v>235</v>
+      </c>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="2:10" ht="216" x14ac:dyDescent="0.3">
@@ -2934,22 +2976,22 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -2958,19 +3000,19 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="1"/>
@@ -2980,19 +3022,19 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I38" s="31"/>
       <c r="J38" s="1"/>
@@ -3002,19 +3044,19 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I39" s="31"/>
       <c r="J39" s="1"/>
@@ -3024,19 +3066,19 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I40" s="31"/>
       <c r="J40" s="1"/>
@@ -3046,19 +3088,19 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I41" s="31"/>
       <c r="J41" s="1"/>
@@ -3068,19 +3110,19 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I42" s="31"/>
       <c r="J42" s="1"/>
@@ -3090,19 +3132,19 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H43" s="30" t="s">
         <v>102</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H43" s="30" t="s">
-        <v>104</v>
       </c>
       <c r="I43" s="31"/>
       <c r="J43" s="1"/>
@@ -3112,19 +3154,19 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I44" s="31"/>
       <c r="J44" s="1"/>
@@ -3134,19 +3176,19 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I45" s="31"/>
       <c r="J45" s="1"/>
@@ -3156,19 +3198,19 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I46" s="31"/>
       <c r="J46" s="1"/>
@@ -3178,19 +3220,19 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I47" s="31"/>
       <c r="J47" s="1"/>
@@ -3200,19 +3242,19 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I48" s="31"/>
       <c r="J48" s="1"/>
@@ -3222,19 +3264,19 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I49" s="31"/>
       <c r="J49" s="1"/>
@@ -3244,22 +3286,22 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I50" s="31" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="J50" s="1"/>
     </row>
@@ -3268,21 +3310,21 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="I51" s="31"/>
+        <v>117</v>
+      </c>
+      <c r="I51" s="30"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
@@ -3299,10 +3341,10 @@
         <v>41</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I52" s="30"/>
       <c r="J52" s="1"/>
@@ -3321,10 +3363,10 @@
         <v>41</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I53" s="30"/>
       <c r="J53" s="1"/>
@@ -3343,10 +3385,10 @@
         <v>41</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I54" s="30"/>
       <c r="J54" s="1"/>
@@ -3365,20 +3407,20 @@
         <v>41</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I55" s="30"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B56" s="29">
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>240</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>129</v>
@@ -3387,32 +3429,32 @@
         <v>41</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>119</v>
+        <v>236</v>
       </c>
       <c r="I56" s="30"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B57" s="29">
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>76</v>
+        <v>239</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>130</v>
+        <v>236</v>
       </c>
       <c r="I57" s="30"/>
       <c r="J57" s="1"/>
@@ -3431,32 +3473,32 @@
         <v>41</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I58" s="30"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B59" s="29">
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="F59" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="I59" s="30"/>
       <c r="J59" s="1"/>
@@ -3466,41 +3508,41 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="F60" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I60" s="30"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B61" s="29">
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H61" s="30" t="s">
-        <v>130</v>
+        <v>236</v>
       </c>
       <c r="I61" s="30"/>
       <c r="J61" s="1"/>
@@ -3510,65 +3552,62 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E62" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="F62" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I62" s="30"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" s="32" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="29">
         <v>61</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="C63" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H63" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="I63" s="30"/>
-      <c r="J63" s="1"/>
+      <c r="G63" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="H63" s="33" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="29">
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="I64" s="30"/>
+        <v>142</v>
+      </c>
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.3">
@@ -3576,21 +3615,20 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H65" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="I65" s="30"/>
+        <v>142</v>
+      </c>
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.3">
@@ -3598,21 +3636,20 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>76</v>
+        <v>145</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I66" s="30"/>
+        <v>142</v>
+      </c>
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.3">
@@ -3620,21 +3657,20 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="F67" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="H67" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I67" s="30"/>
+        <v>142</v>
+      </c>
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.3">
@@ -3645,18 +3681,15 @@
         <v>149</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H68" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I68" s="30"/>
+        <v>190</v>
+      </c>
+      <c r="H68" s="30"/>
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.3">
@@ -3664,21 +3697,18 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H69" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I69" s="30"/>
+        <v>191</v>
+      </c>
+      <c r="H69" s="30"/>
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.3">
@@ -3686,21 +3716,20 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>20</v>
+        <v>155</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="I70" s="30"/>
+        <v>221</v>
+      </c>
       <c r="J70" s="1"/>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.3">
@@ -3708,21 +3737,20 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H71" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="I71" s="30"/>
+        <v>157</v>
+      </c>
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.3">
@@ -3730,21 +3758,20 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>132</v>
+        <v>30</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H72" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="I72" s="30"/>
+        <v>157</v>
+      </c>
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.3">
@@ -3752,21 +3779,20 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>153</v>
+        <v>12</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="I73" s="30"/>
+        <v>157</v>
+      </c>
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.3">
@@ -3774,21 +3800,18 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H74" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="I74" s="30"/>
+        <v>191</v>
+      </c>
+      <c r="H74" s="30"/>
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.3">
@@ -3796,20 +3819,18 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>155</v>
+        <v>79</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H75" s="30" t="s">
-        <v>158</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H75" s="30"/>
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.3">
@@ -3817,20 +3838,18 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H76" s="30" t="s">
-        <v>158</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H76" s="30"/>
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.3">
@@ -3838,20 +3857,18 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H77" s="30" t="s">
-        <v>158</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H77" s="30"/>
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.3">
@@ -3859,20 +3876,18 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H78" s="30" t="s">
-        <v>158</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H78" s="30"/>
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.3">
@@ -3880,20 +3895,18 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="H79" s="30" t="s">
-        <v>158</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H79" s="30"/>
       <c r="J79" s="1"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.3">
@@ -3901,16 +3914,16 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="H80" s="30"/>
       <c r="J80" s="1"/>
@@ -3920,16 +3933,16 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H81" s="30"/>
       <c r="J81" s="1"/>
@@ -3939,16 +3952,16 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>171</v>
+        <v>41</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H82" s="30"/>
       <c r="J82" s="1"/>
@@ -3958,20 +3971,18 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>71</v>
+        <v>174</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H83" s="30" t="s">
-        <v>173</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H83" s="30"/>
       <c r="J83" s="1"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.3">
@@ -3979,20 +3990,18 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>9</v>
+        <v>176</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>30</v>
+        <v>177</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H84" s="30" t="s">
-        <v>173</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H84" s="30"/>
       <c r="J84" s="1"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.3">
@@ -4000,20 +4009,18 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>12</v>
+        <v>178</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H85" s="30" t="s">
-        <v>173</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="H85" s="30"/>
       <c r="J85" s="1"/>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.3">
@@ -4021,16 +4028,16 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>71</v>
+        <v>180</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H86" s="30"/>
       <c r="J86" s="1"/>
@@ -4040,16 +4047,16 @@
         <v>85</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>81</v>
+        <v>36</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H87" s="30"/>
       <c r="J87" s="1"/>
@@ -4059,16 +4066,16 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>59</v>
+        <v>185</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="H88" s="30"/>
       <c r="J88" s="1"/>
@@ -4078,230 +4085,25 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>178</v>
+        <v>229</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>179</v>
+        <v>225</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H89" s="30"/>
-      <c r="J89" s="1"/>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B90" s="29">
-        <v>88</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H90" s="30"/>
-      <c r="J90" s="1"/>
-    </row>
-    <row r="91" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B91" s="29">
-        <v>89</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H91" s="30"/>
-      <c r="J91" s="1"/>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B92" s="29">
-        <v>90</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H92" s="30"/>
-      <c r="J92" s="1"/>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B93" s="29">
-        <v>91</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H93" s="30"/>
-      <c r="J93" s="1"/>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B94" s="29">
-        <v>92</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E94" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G89" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H94" s="30"/>
-      <c r="J94" s="1"/>
-    </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B95" s="29">
-        <v>93</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H95" s="30"/>
-      <c r="J95" s="1"/>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B96" s="29">
-        <v>94</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H96" s="30"/>
-      <c r="J96" s="1"/>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B97" s="29">
-        <v>95</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H97" s="30"/>
-      <c r="J97" s="1"/>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B98" s="29">
-        <v>96</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H98" s="30"/>
-      <c r="J98" s="1"/>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B99" s="29">
-        <v>97</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H99" s="30"/>
-      <c r="J99" s="1"/>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B100" s="29">
-        <v>98</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="H100" s="30"/>
-      <c r="J100" s="1"/>
-    </row>
-    <row r="104" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="H89" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="I89" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
fix the version of: CCBS_DownloadPositionAndDetails
</commit_message>
<xml_diff>
--- a/IA_CCBS_BANK_SIDE/Position/CCBS_DownloadPositionAndDetails.xlsx
+++ b/IA_CCBS_BANK_SIDE/Position/CCBS_DownloadPositionAndDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Deploy\IA\InterfacesGitHub\IA_CCBS_BANK_SIDE\Position\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8030FD8E-7A8B-43EF-9685-3BA1C6DF6B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5FD080-A793-4855-9693-629A00E842E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{68F28061-2ECD-4B0A-AB1D-3A449686159F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="240">
   <si>
     <t>Description</t>
   </si>
@@ -268,9 +268,6 @@
     <t>cb_outint</t>
   </si>
   <si>
-    <t>varchar (200)</t>
-  </si>
-  <si>
     <t>cb_self</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
     <t>cb_status</t>
   </si>
   <si>
-    <t>Customer Id</t>
-  </si>
-  <si>
     <t>cu_id</t>
   </si>
   <si>
@@ -640,9 +634,6 @@
     <t>Version</t>
   </si>
   <si>
-    <t>G4.23.6.0</t>
-  </si>
-  <si>
     <t>Invocation</t>
   </si>
   <si>
@@ -677,9 +668,6 @@
   </si>
   <si>
     <t>i-Apply / Model</t>
-  </si>
-  <si>
-    <t>May 2024</t>
   </si>
   <si>
     <t>It is the account code below the relative mapping is below. For the CurrentAccount, SavingAccount, DepositAccount it is going to be used the code 3 deposit. For CreditCard and DebitCard it is going to be used the code 999 Card
@@ -807,6 +795,12 @@
   </si>
   <si>
     <t>Entity's Expenses Balance</t>
+  </si>
+  <si>
+    <t>May 2025</t>
+  </si>
+  <si>
+    <t>G4.25.5.13</t>
   </si>
 </sst>
 </file>
@@ -970,7 +964,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1065,12 +1059,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
@@ -1078,12 +1066,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1101,6 +1083,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1176,14 +1164,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}" name="Table3" displayName="Table3" ref="B2:I89" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="B2:I89" xr:uid="{0C01A10F-97EF-41BD-8A3D-ACDE7E19B4A2}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D85FC2E3-79A0-45C2-8639-25646ED6A534}" name="seq" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{83E3CCC0-86B9-42D8-98C9-3A75A9998122}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{33920283-5C7A-4D81-82C6-FC077DC9168F}" name="Model" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{21207700-9C5E-49FF-B1F1-B3E80983459F}" name="iApply" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{AEB71BB6-2882-4936-9A74-CF7DC5A067E2}" name="Data Type" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{EE278FB3-8A4A-41A3-82EB-96E212089493}" name="Entity" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{14553218-EA08-43B1-8723-80FF07BE96F7}" name="Notes" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{EC9AF9B7-009D-464A-B823-D133DBB7F12A}" name="i-Apply details" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D85FC2E3-79A0-45C2-8639-25646ED6A534}" name="seq" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{83E3CCC0-86B9-42D8-98C9-3A75A9998122}" name="Description" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{33920283-5C7A-4D81-82C6-FC077DC9168F}" name="Model" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{21207700-9C5E-49FF-B1F1-B3E80983459F}" name="iApply" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{AEB71BB6-2882-4936-9A74-CF7DC5A067E2}" name="Data Type" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{EE278FB3-8A4A-41A3-82EB-96E212089493}" name="Entity" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{14553218-EA08-43B1-8723-80FF07BE96F7}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{EC9AF9B7-009D-464A-B823-D133DBB7F12A}" name="i-Apply details" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1488,7 +1476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB8ACDA-C8F4-4728-9499-8B46BAA74AEA}">
   <dimension ref="B2:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1505,34 +1495,34 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>210</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
@@ -1541,10 +1531,10 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
@@ -1553,18 +1543,18 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
@@ -1577,10 +1567,10 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
@@ -1613,19 +1603,19 @@
   <sheetData>
     <row r="2" spans="2:6" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -1663,7 +1653,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -1680,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>13</v>
@@ -1697,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -2233,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DEFA5D-C6DF-4BEE-A0BF-87172BA2BD41}">
   <dimension ref="B1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2256,13 +2246,13 @@
     </row>
     <row r="2" spans="2:10" s="28" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="29" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -2271,13 +2261,13 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
@@ -2294,7 +2284,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="28"/>
@@ -2314,7 +2304,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -2334,7 +2324,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H5" s="30"/>
       <c r="I5" s="31"/>
@@ -2354,7 +2344,7 @@
         <v>27</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="31"/>
@@ -2374,7 +2364,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="31"/>
@@ -2394,11 +2384,11 @@
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="31" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -2409,18 +2399,18 @@
       <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H9" s="30"/>
       <c r="I9" s="31" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -2438,7 +2428,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H10" s="30"/>
       <c r="I10" s="31"/>
@@ -2458,7 +2448,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H11" s="30"/>
       <c r="I11" s="31"/>
@@ -2478,7 +2468,7 @@
         <v>33</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>38</v>
@@ -2500,7 +2490,7 @@
         <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="31"/>
@@ -2520,7 +2510,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H14" s="30"/>
       <c r="I14" s="31"/>
@@ -2540,7 +2530,7 @@
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="31"/>
@@ -2560,7 +2550,7 @@
         <v>41</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H16" s="30"/>
       <c r="I16" s="31"/>
@@ -2580,7 +2570,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H17" s="30"/>
       <c r="I17" s="31"/>
@@ -2600,7 +2590,7 @@
         <v>41</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H18" s="30"/>
       <c r="I18" s="31"/>
@@ -2620,7 +2610,7 @@
         <v>41</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H19" s="30"/>
       <c r="I19" s="31"/>
@@ -2640,7 +2630,7 @@
         <v>41</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H20" s="30"/>
       <c r="I20" s="31"/>
@@ -2660,7 +2650,7 @@
         <v>59</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H21" s="30"/>
       <c r="I21" s="31"/>
@@ -2680,13 +2670,13 @@
         <v>59</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H22" s="30" t="s">
         <v>62</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="J22" s="1"/>
     </row>
@@ -2704,13 +2694,13 @@
         <v>20</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H23" s="30" t="s">
         <v>65</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J23" s="1"/>
     </row>
@@ -2728,7 +2718,7 @@
         <v>41</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H24" s="30"/>
       <c r="I24" s="31"/>
@@ -2748,7 +2738,7 @@
         <v>41</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H25" s="30" t="s">
         <v>70</v>
@@ -2770,7 +2760,7 @@
         <v>41</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H26" s="30"/>
       <c r="I26" s="31"/>
@@ -2783,15 +2773,6 @@
       <c r="C27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="H27" s="30"/>
       <c r="I27" s="31"/>
       <c r="J27" s="1"/>
@@ -2804,16 +2785,16 @@
         <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I28" s="31"/>
       <c r="J28" s="1"/>
@@ -2823,25 +2804,25 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I29" s="31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J29" s="1"/>
     </row>
@@ -2850,16 +2831,16 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H30" s="30"/>
       <c r="I30" s="31"/>
@@ -2870,16 +2851,16 @@
         <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H31" s="30"/>
       <c r="I31" s="31"/>
@@ -2890,16 +2871,16 @@
         <v>30</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H32" s="30"/>
       <c r="I32" s="31"/>
@@ -2910,16 +2891,16 @@
         <v>31</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H33" s="30"/>
       <c r="I33" s="31"/>
@@ -2939,11 +2920,11 @@
         <v>33</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H34" s="30"/>
       <c r="I34" s="31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J34" s="1"/>
     </row>
@@ -2952,22 +2933,22 @@
         <v>33</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I35" s="31" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="J35" s="1"/>
     </row>
@@ -2976,22 +2957,22 @@
         <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I36" s="31" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -3000,19 +2981,19 @@
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I37" s="31"/>
       <c r="J37" s="1"/>
@@ -3022,19 +3003,19 @@
         <v>36</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I38" s="31"/>
       <c r="J38" s="1"/>
@@ -3044,19 +3025,19 @@
         <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I39" s="31"/>
       <c r="J39" s="1"/>
@@ -3066,19 +3047,19 @@
         <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I40" s="31"/>
       <c r="J40" s="1"/>
@@ -3088,19 +3069,19 @@
         <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I41" s="31"/>
       <c r="J41" s="1"/>
@@ -3110,19 +3091,19 @@
         <v>40</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I42" s="31"/>
       <c r="J42" s="1"/>
@@ -3132,19 +3113,19 @@
         <v>41</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H43" s="30" t="s">
         <v>100</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H43" s="30" t="s">
-        <v>102</v>
       </c>
       <c r="I43" s="31"/>
       <c r="J43" s="1"/>
@@ -3154,19 +3135,19 @@
         <v>42</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I44" s="31"/>
       <c r="J44" s="1"/>
@@ -3176,19 +3157,19 @@
         <v>43</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I45" s="31"/>
       <c r="J45" s="1"/>
@@ -3198,19 +3179,19 @@
         <v>44</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I46" s="31"/>
       <c r="J46" s="1"/>
@@ -3220,19 +3201,19 @@
         <v>45</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I47" s="31"/>
       <c r="J47" s="1"/>
@@ -3242,19 +3223,19 @@
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I48" s="31"/>
       <c r="J48" s="1"/>
@@ -3264,19 +3245,19 @@
         <v>47</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I49" s="31"/>
       <c r="J49" s="1"/>
@@ -3286,22 +3267,22 @@
         <v>48</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I50" s="31" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="J50" s="1"/>
     </row>
@@ -3310,19 +3291,19 @@
         <v>49</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I51" s="30"/>
       <c r="J51" s="1"/>
@@ -3332,19 +3313,19 @@
         <v>50</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I52" s="30"/>
       <c r="J52" s="1"/>
@@ -3354,19 +3335,19 @@
         <v>51</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H53" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I53" s="30"/>
       <c r="J53" s="1"/>
@@ -3376,19 +3357,19 @@
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I54" s="30"/>
       <c r="J54" s="1"/>
@@ -3398,19 +3379,19 @@
         <v>53</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I55" s="30"/>
       <c r="J55" s="1"/>
@@ -3420,19 +3401,19 @@
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I56" s="30"/>
       <c r="J56" s="1"/>
@@ -3442,19 +3423,19 @@
         <v>55</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I57" s="30"/>
       <c r="J57" s="1"/>
@@ -3464,19 +3445,19 @@
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I58" s="30"/>
       <c r="J58" s="1"/>
@@ -3486,19 +3467,19 @@
         <v>57</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H59" s="30" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="I59" s="30"/>
       <c r="J59" s="1"/>
@@ -3508,19 +3489,19 @@
         <v>58</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I60" s="30"/>
       <c r="J60" s="1"/>
@@ -3530,19 +3511,19 @@
         <v>59</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H61" s="30" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I61" s="30"/>
       <c r="J61" s="1"/>
@@ -3552,61 +3533,62 @@
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I62" s="30"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="2:10" s="32" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="29">
         <v>61</v>
       </c>
-      <c r="C63" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="E63" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F63" s="32" t="s">
+      <c r="C63" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G63" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="H63" s="33" t="s">
-        <v>223</v>
-      </c>
+      <c r="G63" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H63" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="J63" s="1"/>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B64" s="29">
         <v>62</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H64" s="30" t="s">
         <v>140</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H64" s="30" t="s">
-        <v>142</v>
       </c>
       <c r="J64" s="1"/>
     </row>
@@ -3615,19 +3597,19 @@
         <v>63</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H65" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J65" s="1"/>
     </row>
@@ -3636,19 +3618,19 @@
         <v>64</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J66" s="1"/>
     </row>
@@ -3657,19 +3639,19 @@
         <v>65</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H67" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J67" s="1"/>
     </row>
@@ -3678,16 +3660,16 @@
         <v>66</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H68" s="30"/>
       <c r="J68" s="1"/>
@@ -3697,16 +3679,16 @@
         <v>67</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H69" s="30"/>
       <c r="J69" s="1"/>
@@ -3716,19 +3698,19 @@
         <v>68</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="G70" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H70" s="30" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="J70" s="1"/>
     </row>
@@ -3740,16 +3722,16 @@
         <v>71</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H71" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J71" s="1"/>
     </row>
@@ -3767,10 +3749,10 @@
         <v>8</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H72" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J72" s="1"/>
     </row>
@@ -3788,10 +3770,10 @@
         <v>14</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H73" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J73" s="1"/>
     </row>
@@ -3803,13 +3785,13 @@
         <v>71</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>46</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H74" s="30"/>
       <c r="J74" s="1"/>
@@ -3819,16 +3801,16 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H75" s="30"/>
       <c r="J75" s="1"/>
@@ -3838,16 +3820,16 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H76" s="30"/>
       <c r="J76" s="1"/>
@@ -3857,16 +3839,16 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H77" s="30"/>
       <c r="J77" s="1"/>
@@ -3876,16 +3858,16 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H78" s="30"/>
       <c r="J78" s="1"/>
@@ -3895,16 +3877,16 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H79" s="30"/>
       <c r="J79" s="1"/>
@@ -3914,16 +3896,16 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H80" s="30"/>
       <c r="J80" s="1"/>
@@ -3933,16 +3915,16 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H81" s="30"/>
       <c r="J81" s="1"/>
@@ -3952,16 +3934,16 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H82" s="30"/>
       <c r="J82" s="1"/>
@@ -3971,16 +3953,16 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H83" s="30"/>
       <c r="J83" s="1"/>
@@ -3990,16 +3972,16 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H84" s="30"/>
       <c r="J84" s="1"/>
@@ -4009,16 +3991,16 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H85" s="30"/>
       <c r="J85" s="1"/>
@@ -4028,16 +4010,16 @@
         <v>84</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H86" s="30"/>
       <c r="J86" s="1"/>
@@ -4050,13 +4032,13 @@
         <v>36</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H87" s="30"/>
       <c r="J87" s="1"/>
@@ -4066,16 +4048,16 @@
         <v>86</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F88" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="G88" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H88" s="30"/>
       <c r="J88" s="1"/>
@@ -4085,22 +4067,22 @@
         <v>87</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G89" s="32" t="s">
-        <v>189</v>
+        <v>222</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="H89" s="30" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="92" spans="2:10" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>